<commit_message>
leitura de linhas da planilha
</commit_message>
<xml_diff>
--- a/orcamento.xlsx
+++ b/orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caio.oliveira\Documents\VSCode\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD48B858-4464-4A52-B24E-0DA06540B392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393B4E1F-70A4-4FF6-8692-CA3C8B7E6350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,9 +409,6 @@
     <t xml:space="preserve"> 6.1 </t>
   </si>
   <si>
-    <t xml:space="preserve"> 6.1.1 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 6.1.2 </t>
   </si>
   <si>
@@ -753,10 +750,13 @@
     <t xml:space="preserve"> 01.03 </t>
   </si>
   <si>
-    <t xml:space="preserve"> 01.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 01.02</t>
+    <t xml:space="preserve"> 01.01.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 01.02.01.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 06.01.01 </t>
   </si>
 </sst>
 </file>
@@ -966,24 +966,24 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1317,8 +1317,8 @@
   </sheetPr>
   <dimension ref="A1:I169"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1338,14 +1338,14 @@
       <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25" t="s">
+      <c r="F1" s="31"/>
+      <c r="G1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="25"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="9" t="s">
         <v>3</v>
       </c>
@@ -1357,14 +1357,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26" t="s">
+      <c r="F2" s="29"/>
+      <c r="G2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="26"/>
+      <c r="H2" s="29"/>
       <c r="I2" s="11" t="s">
         <v>7</v>
       </c>
@@ -1383,17 +1383,17 @@
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
@@ -1443,7 +1443,7 @@
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>21</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>25</v>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>29</v>
@@ -2829,7 +2829,7 @@
     </row>
     <row r="61" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>120</v>
+        <v>235</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>49</v>
@@ -2858,7 +2858,7 @@
     </row>
     <row r="62" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>52</v>
@@ -2887,7 +2887,7 @@
     </row>
     <row r="63" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>55</v>
@@ -2916,7 +2916,7 @@
     </row>
     <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -2933,7 +2933,7 @@
     </row>
     <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>37</v>
@@ -2962,7 +2962,7 @@
     </row>
     <row r="66" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>61</v>
@@ -2991,7 +2991,7 @@
     </row>
     <row r="67" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>64</v>
@@ -3020,7 +3020,7 @@
     </row>
     <row r="68" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>67</v>
@@ -3049,7 +3049,7 @@
     </row>
     <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -3066,7 +3066,7 @@
     </row>
     <row r="70" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>72</v>
@@ -3095,7 +3095,7 @@
     </row>
     <row r="71" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>76</v>
@@ -3124,7 +3124,7 @@
     </row>
     <row r="72" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>79</v>
@@ -3153,7 +3153,7 @@
     </row>
     <row r="73" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>82</v>
@@ -3182,12 +3182,12 @@
     </row>
     <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
@@ -3199,7 +3199,7 @@
     </row>
     <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -3216,7 +3216,7 @@
     </row>
     <row r="76" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>49</v>
@@ -3245,7 +3245,7 @@
     </row>
     <row r="77" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>52</v>
@@ -3274,7 +3274,7 @@
     </row>
     <row r="78" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>55</v>
@@ -3303,7 +3303,7 @@
     </row>
     <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -3320,7 +3320,7 @@
     </row>
     <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>37</v>
@@ -3349,7 +3349,7 @@
     </row>
     <row r="81" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>61</v>
@@ -3378,7 +3378,7 @@
     </row>
     <row r="82" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>64</v>
@@ -3407,7 +3407,7 @@
     </row>
     <row r="83" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>67</v>
@@ -3436,7 +3436,7 @@
     </row>
     <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -3453,7 +3453,7 @@
     </row>
     <row r="85" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>72</v>
@@ -3482,7 +3482,7 @@
     </row>
     <row r="86" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>76</v>
@@ -3511,7 +3511,7 @@
     </row>
     <row r="87" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>79</v>
@@ -3540,7 +3540,7 @@
     </row>
     <row r="88" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>82</v>
@@ -3569,12 +3569,12 @@
     </row>
     <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -3603,7 +3603,7 @@
     </row>
     <row r="91" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>49</v>
@@ -3632,7 +3632,7 @@
     </row>
     <row r="92" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>52</v>
@@ -3661,7 +3661,7 @@
     </row>
     <row r="93" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>55</v>
@@ -3690,7 +3690,7 @@
     </row>
     <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -3707,7 +3707,7 @@
     </row>
     <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>37</v>
@@ -3736,7 +3736,7 @@
     </row>
     <row r="96" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>61</v>
@@ -3765,7 +3765,7 @@
     </row>
     <row r="97" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>64</v>
@@ -3794,7 +3794,7 @@
     </row>
     <row r="98" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>67</v>
@@ -3823,7 +3823,7 @@
     </row>
     <row r="99" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -3840,7 +3840,7 @@
     </row>
     <row r="100" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B100" s="6" t="s">
         <v>72</v>
@@ -3869,7 +3869,7 @@
     </row>
     <row r="101" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>76</v>
@@ -3898,7 +3898,7 @@
     </row>
     <row r="102" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B102" s="6" t="s">
         <v>79</v>
@@ -3927,7 +3927,7 @@
     </row>
     <row r="103" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B103" s="6" t="s">
         <v>82</v>
@@ -3956,12 +3956,12 @@
     </row>
     <row r="104" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
@@ -3973,7 +3973,7 @@
     </row>
     <row r="105" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -3990,7 +3990,7 @@
     </row>
     <row r="106" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>49</v>
@@ -4019,7 +4019,7 @@
     </row>
     <row r="107" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>52</v>
@@ -4048,7 +4048,7 @@
     </row>
     <row r="108" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>55</v>
@@ -4077,7 +4077,7 @@
     </row>
     <row r="109" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -4094,7 +4094,7 @@
     </row>
     <row r="110" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>37</v>
@@ -4123,7 +4123,7 @@
     </row>
     <row r="111" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>61</v>
@@ -4152,7 +4152,7 @@
     </row>
     <row r="112" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>64</v>
@@ -4181,7 +4181,7 @@
     </row>
     <row r="113" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>67</v>
@@ -4210,7 +4210,7 @@
     </row>
     <row r="114" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -4227,7 +4227,7 @@
     </row>
     <row r="115" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B115" s="6" t="s">
         <v>72</v>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="116" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>76</v>
@@ -4285,7 +4285,7 @@
     </row>
     <row r="117" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B117" s="6" t="s">
         <v>79</v>
@@ -4314,7 +4314,7 @@
     </row>
     <row r="118" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B118" s="6" t="s">
         <v>82</v>
@@ -4343,12 +4343,12 @@
     </row>
     <row r="119" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
@@ -4360,7 +4360,7 @@
     </row>
     <row r="120" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -4377,7 +4377,7 @@
     </row>
     <row r="121" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>49</v>
@@ -4406,7 +4406,7 @@
     </row>
     <row r="122" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>52</v>
@@ -4435,7 +4435,7 @@
     </row>
     <row r="123" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>55</v>
@@ -4464,7 +4464,7 @@
     </row>
     <row r="124" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -4481,7 +4481,7 @@
     </row>
     <row r="125" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>37</v>
@@ -4510,7 +4510,7 @@
     </row>
     <row r="126" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>61</v>
@@ -4539,7 +4539,7 @@
     </row>
     <row r="127" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>64</v>
@@ -4568,7 +4568,7 @@
     </row>
     <row r="128" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>67</v>
@@ -4597,7 +4597,7 @@
     </row>
     <row r="129" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -4614,7 +4614,7 @@
     </row>
     <row r="130" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>72</v>
@@ -4643,7 +4643,7 @@
     </row>
     <row r="131" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>76</v>
@@ -4672,7 +4672,7 @@
     </row>
     <row r="132" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>79</v>
@@ -4701,7 +4701,7 @@
     </row>
     <row r="133" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>82</v>
@@ -4730,12 +4730,12 @@
     </row>
     <row r="134" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
       <c r="D134" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E134" s="4"/>
       <c r="F134" s="4"/>
@@ -4747,7 +4747,7 @@
     </row>
     <row r="135" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -4764,7 +4764,7 @@
     </row>
     <row r="136" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>49</v>
@@ -4793,7 +4793,7 @@
     </row>
     <row r="137" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B137" s="6" t="s">
         <v>52</v>
@@ -4822,7 +4822,7 @@
     </row>
     <row r="138" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B138" s="6" t="s">
         <v>55</v>
@@ -4851,7 +4851,7 @@
     </row>
     <row r="139" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
@@ -4868,7 +4868,7 @@
     </row>
     <row r="140" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B140" s="6" t="s">
         <v>37</v>
@@ -4897,7 +4897,7 @@
     </row>
     <row r="141" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B141" s="6" t="s">
         <v>61</v>
@@ -4926,7 +4926,7 @@
     </row>
     <row r="142" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B142" s="6" t="s">
         <v>64</v>
@@ -4955,7 +4955,7 @@
     </row>
     <row r="143" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B143" s="6" t="s">
         <v>67</v>
@@ -4984,7 +4984,7 @@
     </row>
     <row r="144" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
@@ -5001,7 +5001,7 @@
     </row>
     <row r="145" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B145" s="6" t="s">
         <v>72</v>
@@ -5030,7 +5030,7 @@
     </row>
     <row r="146" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B146" s="6" t="s">
         <v>76</v>
@@ -5059,7 +5059,7 @@
     </row>
     <row r="147" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B147" s="6" t="s">
         <v>79</v>
@@ -5088,7 +5088,7 @@
     </row>
     <row r="148" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B148" s="6" t="s">
         <v>82</v>
@@ -5117,12 +5117,12 @@
     </row>
     <row r="149" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
       <c r="D149" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E149" s="4"/>
       <c r="F149" s="4"/>
@@ -5134,7 +5134,7 @@
     </row>
     <row r="150" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -5151,7 +5151,7 @@
     </row>
     <row r="151" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B151" s="6" t="s">
         <v>49</v>
@@ -5180,7 +5180,7 @@
     </row>
     <row r="152" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B152" s="6" t="s">
         <v>52</v>
@@ -5209,7 +5209,7 @@
     </row>
     <row r="153" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B153" s="6" t="s">
         <v>55</v>
@@ -5238,7 +5238,7 @@
     </row>
     <row r="154" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
@@ -5255,7 +5255,7 @@
     </row>
     <row r="155" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B155" s="6" t="s">
         <v>37</v>
@@ -5284,7 +5284,7 @@
     </row>
     <row r="156" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B156" s="6" t="s">
         <v>61</v>
@@ -5313,7 +5313,7 @@
     </row>
     <row r="157" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B157" s="6" t="s">
         <v>64</v>
@@ -5342,7 +5342,7 @@
     </row>
     <row r="158" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B158" s="6" t="s">
         <v>67</v>
@@ -5371,7 +5371,7 @@
     </row>
     <row r="159" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
@@ -5388,7 +5388,7 @@
     </row>
     <row r="160" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B160" s="6" t="s">
         <v>72</v>
@@ -5417,7 +5417,7 @@
     </row>
     <row r="161" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B161" s="6" t="s">
         <v>76</v>
@@ -5446,7 +5446,7 @@
     </row>
     <row r="162" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B162" s="6" t="s">
         <v>79</v>
@@ -5475,7 +5475,7 @@
     </row>
     <row r="163" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B163" s="6" t="s">
         <v>82</v>
@@ -5514,49 +5514,49 @@
       <c r="I164" s="21"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A165" s="27"/>
-      <c r="B165" s="27"/>
-      <c r="C165" s="27"/>
+      <c r="A165" s="28"/>
+      <c r="B165" s="28"/>
+      <c r="C165" s="28"/>
       <c r="D165" s="22"/>
       <c r="E165" s="10"/>
-      <c r="F165" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="G165" s="27"/>
-      <c r="H165" s="28">
+      <c r="F165" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="G165" s="28"/>
+      <c r="H165" s="30">
         <v>1945452.28</v>
       </c>
-      <c r="I165" s="27"/>
+      <c r="I165" s="28"/>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A166" s="27"/>
-      <c r="B166" s="27"/>
-      <c r="C166" s="27"/>
+      <c r="A166" s="28"/>
+      <c r="B166" s="28"/>
+      <c r="C166" s="28"/>
       <c r="D166" s="22"/>
       <c r="E166" s="10"/>
-      <c r="F166" s="26" t="s">
-        <v>230</v>
-      </c>
-      <c r="G166" s="27"/>
-      <c r="H166" s="28">
+      <c r="F166" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="G166" s="28"/>
+      <c r="H166" s="30">
         <v>0</v>
       </c>
-      <c r="I166" s="27"/>
+      <c r="I166" s="28"/>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A167" s="27"/>
-      <c r="B167" s="27"/>
-      <c r="C167" s="27"/>
+      <c r="A167" s="28"/>
+      <c r="B167" s="28"/>
+      <c r="C167" s="28"/>
       <c r="D167" s="22"/>
       <c r="E167" s="10"/>
-      <c r="F167" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="G167" s="27"/>
-      <c r="H167" s="28">
+      <c r="F167" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="G167" s="28"/>
+      <c r="H167" s="30">
         <v>1945452.28</v>
       </c>
-      <c r="I167" s="27"/>
+      <c r="I167" s="28"/>
     </row>
     <row r="168" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="10"/>
@@ -5570,20 +5570,27 @@
       <c r="I168" s="23"/>
     </row>
     <row r="169" spans="1:9" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="29" t="s">
-        <v>232</v>
-      </c>
-      <c r="B169" s="30"/>
-      <c r="C169" s="30"/>
-      <c r="D169" s="30"/>
-      <c r="E169" s="30"/>
-      <c r="F169" s="30"/>
-      <c r="G169" s="30"/>
-      <c r="H169" s="30"/>
-      <c r="I169" s="30"/>
+      <c r="A169" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="B169" s="26"/>
+      <c r="C169" s="26"/>
+      <c r="D169" s="26"/>
+      <c r="E169" s="26"/>
+      <c r="F169" s="26"/>
+      <c r="G169" s="26"/>
+      <c r="H169" s="26"/>
+      <c r="I169" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A167:C167"/>
+    <mergeCell ref="F167:G167"/>
+    <mergeCell ref="H167:I167"/>
     <mergeCell ref="A169:I169"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A165:C165"/>
@@ -5592,13 +5599,6 @@
     <mergeCell ref="A166:C166"/>
     <mergeCell ref="F166:G166"/>
     <mergeCell ref="H166:I166"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A167:C167"/>
-    <mergeCell ref="F167:G167"/>
-    <mergeCell ref="H167:I167"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
formatador da coluna bancos
</commit_message>
<xml_diff>
--- a/orcamento.xlsx
+++ b/orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caio.oliveira\Documents\VSCode\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393B4E1F-70A4-4FF6-8692-CA3C8B7E6350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44AB73CB-650F-4F81-B277-A1D5D21A8457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="240">
   <si>
     <t>Obra</t>
   </si>
@@ -757,6 +757,18 @@
   </si>
   <si>
     <t xml:space="preserve"> 06.01.01 </t>
+  </si>
+  <si>
+    <t>SINAPI-C</t>
+  </si>
+  <si>
+    <t>sinapi</t>
+  </si>
+  <si>
+    <t>SINAPI-I</t>
+  </si>
+  <si>
+    <t>sinapi-i</t>
   </si>
 </sst>
 </file>
@@ -966,24 +978,24 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1317,8 +1329,8 @@
   </sheetPr>
   <dimension ref="A1:I169"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1338,14 +1350,14 @@
       <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="31"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="9" t="s">
         <v>3</v>
       </c>
@@ -1357,14 +1369,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29" t="s">
+      <c r="F2" s="26"/>
+      <c r="G2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="29"/>
+      <c r="H2" s="26"/>
       <c r="I2" s="11" t="s">
         <v>7</v>
       </c>
@@ -1383,17 +1395,17 @@
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
@@ -1478,7 +1490,7 @@
         <v>25</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>26</v>
+        <v>236</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>27</v>
@@ -1507,7 +1519,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>26</v>
+        <v>237</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>30</v>
@@ -1553,7 +1565,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>26</v>
+        <v>238</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>35</v>
@@ -1611,7 +1623,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>26</v>
+        <v>239</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>43</v>
@@ -5514,49 +5526,49 @@
       <c r="I164" s="21"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A165" s="28"/>
-      <c r="B165" s="28"/>
-      <c r="C165" s="28"/>
+      <c r="A165" s="27"/>
+      <c r="B165" s="27"/>
+      <c r="C165" s="27"/>
       <c r="D165" s="22"/>
       <c r="E165" s="10"/>
-      <c r="F165" s="29" t="s">
+      <c r="F165" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="G165" s="28"/>
-      <c r="H165" s="30">
+      <c r="G165" s="27"/>
+      <c r="H165" s="28">
         <v>1945452.28</v>
       </c>
-      <c r="I165" s="28"/>
+      <c r="I165" s="27"/>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A166" s="28"/>
-      <c r="B166" s="28"/>
-      <c r="C166" s="28"/>
+      <c r="A166" s="27"/>
+      <c r="B166" s="27"/>
+      <c r="C166" s="27"/>
       <c r="D166" s="22"/>
       <c r="E166" s="10"/>
-      <c r="F166" s="29" t="s">
+      <c r="F166" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="G166" s="28"/>
-      <c r="H166" s="30">
+      <c r="G166" s="27"/>
+      <c r="H166" s="28">
         <v>0</v>
       </c>
-      <c r="I166" s="28"/>
+      <c r="I166" s="27"/>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A167" s="28"/>
-      <c r="B167" s="28"/>
-      <c r="C167" s="28"/>
+      <c r="A167" s="27"/>
+      <c r="B167" s="27"/>
+      <c r="C167" s="27"/>
       <c r="D167" s="22"/>
       <c r="E167" s="10"/>
-      <c r="F167" s="29" t="s">
+      <c r="F167" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="G167" s="28"/>
-      <c r="H167" s="30">
+      <c r="G167" s="27"/>
+      <c r="H167" s="28">
         <v>1945452.28</v>
       </c>
-      <c r="I167" s="28"/>
+      <c r="I167" s="27"/>
     </row>
     <row r="168" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="10"/>
@@ -5570,27 +5582,20 @@
       <c r="I168" s="23"/>
     </row>
     <row r="169" spans="1:9" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="25" t="s">
+      <c r="A169" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="B169" s="26"/>
-      <c r="C169" s="26"/>
-      <c r="D169" s="26"/>
-      <c r="E169" s="26"/>
-      <c r="F169" s="26"/>
-      <c r="G169" s="26"/>
-      <c r="H169" s="26"/>
-      <c r="I169" s="26"/>
+      <c r="B169" s="30"/>
+      <c r="C169" s="30"/>
+      <c r="D169" s="30"/>
+      <c r="E169" s="30"/>
+      <c r="F169" s="30"/>
+      <c r="G169" s="30"/>
+      <c r="H169" s="30"/>
+      <c r="I169" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A167:C167"/>
-    <mergeCell ref="F167:G167"/>
-    <mergeCell ref="H167:I167"/>
     <mergeCell ref="A169:I169"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A165:C165"/>
@@ -5599,6 +5604,13 @@
     <mergeCell ref="A166:C166"/>
     <mergeCell ref="F166:G166"/>
     <mergeCell ref="H166:I166"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A167:C167"/>
+    <mergeCell ref="F167:G167"/>
+    <mergeCell ref="H167:I167"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
otimização do código + criação do arquivo func
</commit_message>
<xml_diff>
--- a/orcamento.xlsx
+++ b/orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caio.oliveira\Documents\VSCode\Python\planiha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F645B6-F610-4CA5-B1B2-E8F7B023AE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74ABA879-33F8-41B4-B242-EE369F3C4A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -738,12 +738,6 @@
     <t xml:space="preserve"> 01.03 </t>
   </si>
   <si>
-    <t xml:space="preserve"> 01.01.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 01.02.01.03</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 06.01.01 </t>
   </si>
   <si>
@@ -766,6 +760,12 @@
   </si>
   <si>
     <t>0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 01.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 01.02.01</t>
   </si>
 </sst>
 </file>
@@ -978,24 +978,24 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1350,14 +1350,14 @@
       <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32" t="s">
+      <c r="F1" s="26"/>
+      <c r="G1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="32"/>
+      <c r="H1" s="26"/>
       <c r="I1" s="9" t="s">
         <v>3</v>
       </c>
@@ -1369,14 +1369,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="27"/>
+      <c r="G2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="30"/>
+      <c r="H2" s="27"/>
       <c r="I2" s="11" t="s">
         <v>7</v>
       </c>
@@ -1395,17 +1395,17 @@
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
@@ -1455,13 +1455,13 @@
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>22</v>
@@ -1484,13 +1484,13 @@
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>230</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>238</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>232</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>25</v>
@@ -1519,7 +1519,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>28</v>
@@ -1562,10 +1562,10 @@
         <v>31</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>32</v>
@@ -1623,7 +1623,7 @@
         <v>894</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>39</v>
@@ -2841,7 +2841,7 @@
     </row>
     <row r="61" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>45</v>
@@ -5526,49 +5526,49 @@
       <c r="I164" s="21"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A165" s="29"/>
-      <c r="B165" s="29"/>
-      <c r="C165" s="29"/>
+      <c r="A165" s="28"/>
+      <c r="B165" s="28"/>
+      <c r="C165" s="28"/>
       <c r="D165" s="22"/>
       <c r="E165" s="10"/>
-      <c r="F165" s="30" t="s">
+      <c r="F165" s="27" t="s">
         <v>224</v>
       </c>
-      <c r="G165" s="29"/>
-      <c r="H165" s="31">
+      <c r="G165" s="28"/>
+      <c r="H165" s="29">
         <v>1945452.28</v>
       </c>
-      <c r="I165" s="29"/>
+      <c r="I165" s="28"/>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A166" s="29"/>
-      <c r="B166" s="29"/>
-      <c r="C166" s="29"/>
+      <c r="A166" s="28"/>
+      <c r="B166" s="28"/>
+      <c r="C166" s="28"/>
       <c r="D166" s="22"/>
       <c r="E166" s="10"/>
-      <c r="F166" s="30" t="s">
+      <c r="F166" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="G166" s="29"/>
-      <c r="H166" s="31">
+      <c r="G166" s="28"/>
+      <c r="H166" s="29">
         <v>0</v>
       </c>
-      <c r="I166" s="29"/>
+      <c r="I166" s="28"/>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A167" s="29"/>
-      <c r="B167" s="29"/>
-      <c r="C167" s="29"/>
+      <c r="A167" s="28"/>
+      <c r="B167" s="28"/>
+      <c r="C167" s="28"/>
       <c r="D167" s="22"/>
       <c r="E167" s="10"/>
-      <c r="F167" s="30" t="s">
+      <c r="F167" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="G167" s="29"/>
-      <c r="H167" s="31">
+      <c r="G167" s="28"/>
+      <c r="H167" s="29">
         <v>1945452.28</v>
       </c>
-      <c r="I167" s="29"/>
+      <c r="I167" s="28"/>
     </row>
     <row r="168" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="10"/>
@@ -5582,27 +5582,20 @@
       <c r="I168" s="23"/>
     </row>
     <row r="169" spans="1:9" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="26" t="s">
+      <c r="A169" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="B169" s="27"/>
-      <c r="C169" s="27"/>
-      <c r="D169" s="27"/>
-      <c r="E169" s="27"/>
-      <c r="F169" s="27"/>
-      <c r="G169" s="27"/>
-      <c r="H169" s="27"/>
-      <c r="I169" s="27"/>
+      <c r="B169" s="31"/>
+      <c r="C169" s="31"/>
+      <c r="D169" s="31"/>
+      <c r="E169" s="31"/>
+      <c r="F169" s="31"/>
+      <c r="G169" s="31"/>
+      <c r="H169" s="31"/>
+      <c r="I169" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A167:C167"/>
-    <mergeCell ref="F167:G167"/>
-    <mergeCell ref="H167:I167"/>
     <mergeCell ref="A169:I169"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A165:C165"/>
@@ -5611,6 +5604,13 @@
     <mergeCell ref="A166:C166"/>
     <mergeCell ref="F166:G166"/>
     <mergeCell ref="H166:I166"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A167:C167"/>
+    <mergeCell ref="F167:G167"/>
+    <mergeCell ref="H167:I167"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
comps e ins dos bancos sicro e cpos
</commit_message>
<xml_diff>
--- a/orcamento.xlsx
+++ b/orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caio.oliveira\Documents\VSCode\Python\planiha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9D55BE-344D-4DE6-B143-030CCD5FFF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53545B7C-9499-4618-8187-07C9711FD434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="246">
   <si>
     <t>Obra</t>
   </si>
@@ -157,9 +157,6 @@
     <t xml:space="preserve"> 2.3 </t>
   </si>
   <si>
-    <t>ALVENARIA DE BLOCOS DE CONCRETO ESTRUTURAL 14X19X29 CM, (ESPESSURA 14 CM) FBK = 14,0 MPA, PARA PAREDES COM ÁREA LÍQUIDA MAIOR OU IGUAL A 6M², COM VÃOS, UTILIZANDO COLHER DE PEDREIRO. AF_12/2014</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 3 </t>
   </si>
   <si>
@@ -738,9 +735,6 @@
     <t>SINAPI-I</t>
   </si>
   <si>
-    <t>sinapi-i</t>
-  </si>
-  <si>
     <t>sbc</t>
   </si>
   <si>
@@ -766,6 +760,33 @@
   </si>
   <si>
     <t>87</t>
+  </si>
+  <si>
+    <t>SICRO</t>
+  </si>
+  <si>
+    <t>3009304</t>
+  </si>
+  <si>
+    <t>Trilho TR45, comprimento de 120 m (TLS), sobre dormente de concreto, bitola mista, taxa de dormentação de 1.667 un/km, tala de junção de 6 furos e fixação elástica Pandrol - posicionamento e assentamento mecanizado</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>Solda elétrica por caldeamento para trilho TR45, comprimento de até 24 m, em via com dormente de madeira para formação de barra ou trilho longo soldado</t>
+  </si>
+  <si>
+    <t>30093</t>
+  </si>
+  <si>
+    <t>O.05.000.062408</t>
+  </si>
+  <si>
+    <t>Abraçadeira dentada para travamento em ferro fundido, predial SMU DN= 50 mm</t>
+  </si>
+  <si>
+    <t>un</t>
   </si>
 </sst>
 </file>
@@ -999,24 +1020,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1350,8 +1371,8 @@
   </sheetPr>
   <dimension ref="A1:I169"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1372,14 +1393,14 @@
       <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33" t="s">
+      <c r="F1" s="39"/>
+      <c r="G1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="33"/>
+      <c r="H1" s="39"/>
       <c r="I1" s="9" t="s">
         <v>3</v>
       </c>
@@ -1391,14 +1412,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34" t="s">
+      <c r="F2" s="37"/>
+      <c r="G2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="34"/>
+      <c r="H2" s="37"/>
       <c r="I2" s="11" t="s">
         <v>7</v>
       </c>
@@ -1417,17 +1438,17 @@
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
@@ -1477,16 +1498,16 @@
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>232</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>21</v>
@@ -1506,16 +1527,16 @@
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>23</v>
@@ -1535,13 +1556,13 @@
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>25</v>
@@ -1584,10 +1605,10 @@
         <v>28</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>29</v>
@@ -1641,17 +1662,17 @@
       <c r="A13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="25">
-        <v>894</v>
+      <c r="B13" s="25" t="s">
+        <v>243</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>229</v>
+        <v>32</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>36</v>
+        <v>244</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>23</v>
+        <v>245</v>
       </c>
       <c r="F13" s="6">
         <v>85.51</v>
@@ -1668,12 +1689,12 @@
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="30"/>
       <c r="C14" s="4"/>
       <c r="D14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -1685,12 +1706,12 @@
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="29"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1702,57 +1723,55 @@
     </row>
     <row r="16" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>42</v>
+        <v>238</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>22</v>
+        <v>237</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>43</v>
+        <v>239</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>23</v>
+        <v>240</v>
       </c>
       <c r="F16" s="6">
-        <v>242.85</v>
+        <v>1</v>
       </c>
       <c r="G16" s="17">
-        <v>150.88</v>
+        <v>1453769.69</v>
       </c>
       <c r="H16" s="17">
-        <v>150.88</v>
-      </c>
-      <c r="I16" s="18">
-        <v>36641.199999999997</v>
-      </c>
+        <v>1453769.69</v>
+      </c>
+      <c r="I16" s="18"/>
     </row>
     <row r="17" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>45</v>
+        <v>242</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>22</v>
+        <v>237</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>46</v>
+        <v>241</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F17" s="6">
-        <v>5.39</v>
+        <v>1</v>
       </c>
       <c r="G17" s="17">
-        <v>64.400000000000006</v>
+        <v>234.78</v>
       </c>
       <c r="H17" s="17">
-        <v>64.400000000000006</v>
+        <v>234.78</v>
       </c>
       <c r="I17" s="18">
         <v>347.11</v>
@@ -1760,16 +1779,16 @@
     </row>
     <row r="18" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="C18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>23</v>
@@ -1789,12 +1808,12 @@
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="30"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1806,7 +1825,7 @@
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>31</v>
@@ -1835,16 +1854,16 @@
     </row>
     <row r="21" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="C21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>23</v>
@@ -1864,16 +1883,16 @@
     </row>
     <row r="22" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="C22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>23</v>
@@ -1893,16 +1912,16 @@
     </row>
     <row r="23" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="C23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>23</v>
@@ -1922,12 +1941,12 @@
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="30"/>
       <c r="C24" s="4"/>
       <c r="D24" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -1939,19 +1958,19 @@
     </row>
     <row r="25" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="C25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="7" t="s">
+      <c r="E25" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="F25" s="6">
         <v>12</v>
@@ -1968,16 +1987,16 @@
     </row>
     <row r="26" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="C26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>23</v>
@@ -1997,16 +2016,16 @@
     </row>
     <row r="27" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="C27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>23</v>
@@ -2026,19 +2045,19 @@
     </row>
     <row r="28" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="C28" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="7" t="s">
+      <c r="E28" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="F28" s="6">
         <v>3.6</v>
@@ -2055,12 +2074,12 @@
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B29" s="30"/>
       <c r="C29" s="4"/>
       <c r="D29" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -2072,12 +2091,12 @@
     </row>
     <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="29"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -2089,16 +2108,16 @@
     </row>
     <row r="31" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>23</v>
@@ -2118,16 +2137,16 @@
     </row>
     <row r="32" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>23</v>
@@ -2147,16 +2166,16 @@
     </row>
     <row r="33" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B33" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>23</v>
@@ -2176,12 +2195,12 @@
     </row>
     <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="30"/>
       <c r="C34" s="4"/>
       <c r="D34" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -2193,7 +2212,7 @@
     </row>
     <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="25" t="s">
         <v>31</v>
@@ -2222,16 +2241,16 @@
     </row>
     <row r="36" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B36" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>23</v>
@@ -2251,16 +2270,16 @@
     </row>
     <row r="37" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B37" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>23</v>
@@ -2280,16 +2299,16 @@
     </row>
     <row r="38" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>23</v>
@@ -2309,12 +2328,12 @@
     </row>
     <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B39" s="30"/>
       <c r="C39" s="4"/>
       <c r="D39" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -2326,19 +2345,19 @@
     </row>
     <row r="40" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B40" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="7" t="s">
+      <c r="E40" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="F40" s="6">
         <v>12</v>
@@ -2355,16 +2374,16 @@
     </row>
     <row r="41" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B41" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>23</v>
@@ -2384,16 +2403,16 @@
     </row>
     <row r="42" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B42" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>23</v>
@@ -2413,19 +2432,19 @@
     </row>
     <row r="43" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B43" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D43" s="7" t="s">
+      <c r="E43" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="F43" s="6">
         <v>3.6</v>
@@ -2442,12 +2461,12 @@
     </row>
     <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B44" s="30"/>
       <c r="C44" s="4"/>
       <c r="D44" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -2459,12 +2478,12 @@
     </row>
     <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B45" s="29"/>
       <c r="C45" s="2"/>
       <c r="D45" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
@@ -2476,16 +2495,16 @@
     </row>
     <row r="46" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B46" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>23</v>
@@ -2505,16 +2524,16 @@
     </row>
     <row r="47" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B47" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>23</v>
@@ -2534,16 +2553,16 @@
     </row>
     <row r="48" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B48" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>23</v>
@@ -2563,12 +2582,12 @@
     </row>
     <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B49" s="30"/>
       <c r="C49" s="4"/>
       <c r="D49" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -2580,7 +2599,7 @@
     </row>
     <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B50" s="25" t="s">
         <v>31</v>
@@ -2609,16 +2628,16 @@
     </row>
     <row r="51" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B51" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>23</v>
@@ -2638,16 +2657,16 @@
     </row>
     <row r="52" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B52" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>23</v>
@@ -2667,16 +2686,16 @@
     </row>
     <row r="53" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B53" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>23</v>
@@ -2696,12 +2715,12 @@
     </row>
     <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B54" s="30"/>
       <c r="C54" s="4"/>
       <c r="D54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -2713,19 +2732,19 @@
     </row>
     <row r="55" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B55" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D55" s="7" t="s">
+      <c r="E55" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="F55" s="6">
         <v>12</v>
@@ -2742,16 +2761,16 @@
     </row>
     <row r="56" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B56" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>23</v>
@@ -2771,16 +2790,16 @@
     </row>
     <row r="57" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B57" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>23</v>
@@ -2800,19 +2819,19 @@
     </row>
     <row r="58" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B58" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C58" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D58" s="7" t="s">
+      <c r="E58" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="F58" s="6">
         <v>3.6</v>
@@ -2829,12 +2848,12 @@
     </row>
     <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B59" s="30"/>
       <c r="C59" s="4"/>
       <c r="D59" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -2846,12 +2865,12 @@
     </row>
     <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B60" s="29"/>
       <c r="C60" s="2"/>
       <c r="D60" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
@@ -2863,16 +2882,16 @@
     </row>
     <row r="61" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B61" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>23</v>
@@ -2892,16 +2911,16 @@
     </row>
     <row r="62" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B62" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>23</v>
@@ -2921,16 +2940,16 @@
     </row>
     <row r="63" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B63" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>23</v>
@@ -2950,12 +2969,12 @@
     </row>
     <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B64" s="30"/>
       <c r="C64" s="4"/>
       <c r="D64" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
@@ -2967,7 +2986,7 @@
     </row>
     <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B65" s="25" t="s">
         <v>31</v>
@@ -2996,16 +3015,16 @@
     </row>
     <row r="66" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B66" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>23</v>
@@ -3025,16 +3044,16 @@
     </row>
     <row r="67" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B67" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>23</v>
@@ -3054,16 +3073,16 @@
     </row>
     <row r="68" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B68" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D68" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>23</v>
@@ -3083,12 +3102,12 @@
     </row>
     <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B69" s="30"/>
       <c r="C69" s="4"/>
       <c r="D69" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
@@ -3100,19 +3119,19 @@
     </row>
     <row r="70" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B70" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D70" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C70" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D70" s="7" t="s">
+      <c r="E70" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="F70" s="6">
         <v>12</v>
@@ -3129,16 +3148,16 @@
     </row>
     <row r="71" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B71" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D71" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>23</v>
@@ -3158,16 +3177,16 @@
     </row>
     <row r="72" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B72" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>23</v>
@@ -3187,19 +3206,19 @@
     </row>
     <row r="73" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B73" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D73" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C73" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D73" s="7" t="s">
+      <c r="E73" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="F73" s="6">
         <v>3.6</v>
@@ -3216,12 +3235,12 @@
     </row>
     <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B74" s="30"/>
       <c r="C74" s="4"/>
       <c r="D74" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
@@ -3233,12 +3252,12 @@
     </row>
     <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B75" s="29"/>
       <c r="C75" s="2"/>
       <c r="D75" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -3250,16 +3269,16 @@
     </row>
     <row r="76" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B76" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D76" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>23</v>
@@ -3279,16 +3298,16 @@
     </row>
     <row r="77" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B77" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D77" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>23</v>
@@ -3308,16 +3327,16 @@
     </row>
     <row r="78" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B78" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D78" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>23</v>
@@ -3337,12 +3356,12 @@
     </row>
     <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B79" s="30"/>
       <c r="C79" s="4"/>
       <c r="D79" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
@@ -3354,7 +3373,7 @@
     </row>
     <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B80" s="25" t="s">
         <v>31</v>
@@ -3383,16 +3402,16 @@
     </row>
     <row r="81" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B81" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D81" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>23</v>
@@ -3412,16 +3431,16 @@
     </row>
     <row r="82" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B82" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D82" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>23</v>
@@ -3441,16 +3460,16 @@
     </row>
     <row r="83" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B83" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D83" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>23</v>
@@ -3470,12 +3489,12 @@
     </row>
     <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B84" s="30"/>
       <c r="C84" s="4"/>
       <c r="D84" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
@@ -3487,19 +3506,19 @@
     </row>
     <row r="85" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B85" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D85" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C85" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D85" s="7" t="s">
+      <c r="E85" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="F85" s="6">
         <v>12</v>
@@ -3516,16 +3535,16 @@
     </row>
     <row r="86" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B86" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D86" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>23</v>
@@ -3545,16 +3564,16 @@
     </row>
     <row r="87" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B87" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D87" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>23</v>
@@ -3574,19 +3593,19 @@
     </row>
     <row r="88" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B88" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D88" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C88" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D88" s="7" t="s">
+      <c r="E88" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="F88" s="6">
         <v>3.6</v>
@@ -3603,12 +3622,12 @@
     </row>
     <row r="89" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B89" s="30"/>
       <c r="C89" s="4"/>
       <c r="D89" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
@@ -3620,12 +3639,12 @@
     </row>
     <row r="90" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B90" s="29"/>
       <c r="C90" s="2"/>
       <c r="D90" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
@@ -3637,16 +3656,16 @@
     </row>
     <row r="91" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B91" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D91" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>23</v>
@@ -3666,16 +3685,16 @@
     </row>
     <row r="92" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B92" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D92" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>23</v>
@@ -3695,16 +3714,16 @@
     </row>
     <row r="93" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B93" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D93" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>23</v>
@@ -3724,12 +3743,12 @@
     </row>
     <row r="94" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B94" s="30"/>
       <c r="C94" s="4"/>
       <c r="D94" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
@@ -3741,7 +3760,7 @@
     </row>
     <row r="95" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B95" s="25" t="s">
         <v>31</v>
@@ -3770,16 +3789,16 @@
     </row>
     <row r="96" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B96" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D96" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="E96" s="6" t="s">
         <v>23</v>
@@ -3799,16 +3818,16 @@
     </row>
     <row r="97" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B97" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D97" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>23</v>
@@ -3828,16 +3847,16 @@
     </row>
     <row r="98" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B98" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D98" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D98" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="E98" s="6" t="s">
         <v>23</v>
@@ -3857,12 +3876,12 @@
     </row>
     <row r="99" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B99" s="30"/>
       <c r="C99" s="4"/>
       <c r="D99" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
@@ -3874,19 +3893,19 @@
     </row>
     <row r="100" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B100" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D100" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C100" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D100" s="7" t="s">
+      <c r="E100" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="E100" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="F100" s="6">
         <v>12</v>
@@ -3903,16 +3922,16 @@
     </row>
     <row r="101" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B101" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D101" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D101" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="E101" s="6" t="s">
         <v>23</v>
@@ -3932,16 +3951,16 @@
     </row>
     <row r="102" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B102" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D102" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D102" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="E102" s="6" t="s">
         <v>23</v>
@@ -3961,19 +3980,19 @@
     </row>
     <row r="103" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B103" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D103" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C103" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D103" s="7" t="s">
+      <c r="E103" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="F103" s="6">
         <v>3.6</v>
@@ -3990,12 +4009,12 @@
     </row>
     <row r="104" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B104" s="30"/>
       <c r="C104" s="4"/>
       <c r="D104" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
@@ -4007,12 +4026,12 @@
     </row>
     <row r="105" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B105" s="29"/>
       <c r="C105" s="2"/>
       <c r="D105" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -4024,16 +4043,16 @@
     </row>
     <row r="106" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B106" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D106" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="E106" s="6" t="s">
         <v>23</v>
@@ -4053,16 +4072,16 @@
     </row>
     <row r="107" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B107" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D107" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="C107" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D107" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="E107" s="6" t="s">
         <v>23</v>
@@ -4082,16 +4101,16 @@
     </row>
     <row r="108" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B108" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D108" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="C108" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D108" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>23</v>
@@ -4111,12 +4130,12 @@
     </row>
     <row r="109" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B109" s="30"/>
       <c r="C109" s="4"/>
       <c r="D109" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
@@ -4128,7 +4147,7 @@
     </row>
     <row r="110" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B110" s="25" t="s">
         <v>31</v>
@@ -4157,16 +4176,16 @@
     </row>
     <row r="111" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B111" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D111" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D111" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="E111" s="6" t="s">
         <v>23</v>
@@ -4186,16 +4205,16 @@
     </row>
     <row r="112" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B112" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D112" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="C112" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D112" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="E112" s="6" t="s">
         <v>23</v>
@@ -4215,16 +4234,16 @@
     </row>
     <row r="113" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B113" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D113" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D113" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="E113" s="6" t="s">
         <v>23</v>
@@ -4244,12 +4263,12 @@
     </row>
     <row r="114" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B114" s="30"/>
       <c r="C114" s="4"/>
       <c r="D114" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
@@ -4261,19 +4280,19 @@
     </row>
     <row r="115" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B115" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D115" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C115" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D115" s="7" t="s">
+      <c r="E115" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="E115" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="F115" s="6">
         <v>12</v>
@@ -4290,16 +4309,16 @@
     </row>
     <row r="116" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B116" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D116" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D116" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="E116" s="6" t="s">
         <v>23</v>
@@ -4319,16 +4338,16 @@
     </row>
     <row r="117" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B117" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D117" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C117" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D117" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="E117" s="6" t="s">
         <v>23</v>
@@ -4348,19 +4367,19 @@
     </row>
     <row r="118" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B118" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D118" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C118" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D118" s="7" t="s">
+      <c r="E118" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="E118" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="F118" s="6">
         <v>3.6</v>
@@ -4377,12 +4396,12 @@
     </row>
     <row r="119" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B119" s="30"/>
       <c r="C119" s="4"/>
       <c r="D119" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
@@ -4394,12 +4413,12 @@
     </row>
     <row r="120" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B120" s="29"/>
       <c r="C120" s="2"/>
       <c r="D120" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
@@ -4411,16 +4430,16 @@
     </row>
     <row r="121" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B121" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D121" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="C121" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D121" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="E121" s="6" t="s">
         <v>23</v>
@@ -4440,16 +4459,16 @@
     </row>
     <row r="122" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B122" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D122" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D122" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="E122" s="6" t="s">
         <v>23</v>
@@ -4469,16 +4488,16 @@
     </row>
     <row r="123" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B123" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D123" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D123" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="E123" s="6" t="s">
         <v>23</v>
@@ -4498,12 +4517,12 @@
     </row>
     <row r="124" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B124" s="30"/>
       <c r="C124" s="4"/>
       <c r="D124" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E124" s="4"/>
       <c r="F124" s="4"/>
@@ -4515,7 +4534,7 @@
     </row>
     <row r="125" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B125" s="25" t="s">
         <v>31</v>
@@ -4544,16 +4563,16 @@
     </row>
     <row r="126" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B126" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D126" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C126" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D126" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="E126" s="6" t="s">
         <v>23</v>
@@ -4573,16 +4592,16 @@
     </row>
     <row r="127" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B127" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D127" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="C127" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D127" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="E127" s="6" t="s">
         <v>23</v>
@@ -4602,16 +4621,16 @@
     </row>
     <row r="128" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B128" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D128" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C128" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D128" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="E128" s="6" t="s">
         <v>23</v>
@@ -4631,12 +4650,12 @@
     </row>
     <row r="129" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B129" s="30"/>
       <c r="C129" s="4"/>
       <c r="D129" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E129" s="4"/>
       <c r="F129" s="4"/>
@@ -4648,19 +4667,19 @@
     </row>
     <row r="130" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B130" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D130" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C130" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D130" s="7" t="s">
+      <c r="E130" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="E130" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="F130" s="6">
         <v>12</v>
@@ -4677,16 +4696,16 @@
     </row>
     <row r="131" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B131" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D131" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D131" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="E131" s="6" t="s">
         <v>23</v>
@@ -4706,16 +4725,16 @@
     </row>
     <row r="132" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B132" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D132" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C132" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D132" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="E132" s="6" t="s">
         <v>23</v>
@@ -4735,19 +4754,19 @@
     </row>
     <row r="133" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B133" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D133" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C133" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D133" s="7" t="s">
+      <c r="E133" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="E133" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="F133" s="6">
         <v>3.6</v>
@@ -4764,12 +4783,12 @@
     </row>
     <row r="134" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B134" s="30"/>
       <c r="C134" s="4"/>
       <c r="D134" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E134" s="4"/>
       <c r="F134" s="4"/>
@@ -4781,12 +4800,12 @@
     </row>
     <row r="135" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B135" s="29"/>
       <c r="C135" s="2"/>
       <c r="D135" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
@@ -4798,16 +4817,16 @@
     </row>
     <row r="136" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B136" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D136" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="C136" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D136" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="E136" s="6" t="s">
         <v>23</v>
@@ -4827,16 +4846,16 @@
     </row>
     <row r="137" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B137" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D137" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="C137" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D137" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="E137" s="6" t="s">
         <v>23</v>
@@ -4856,16 +4875,16 @@
     </row>
     <row r="138" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B138" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D138" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="C138" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D138" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="E138" s="6" t="s">
         <v>23</v>
@@ -4885,12 +4904,12 @@
     </row>
     <row r="139" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B139" s="30"/>
       <c r="C139" s="4"/>
       <c r="D139" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E139" s="4"/>
       <c r="F139" s="4"/>
@@ -4902,7 +4921,7 @@
     </row>
     <row r="140" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B140" s="25" t="s">
         <v>31</v>
@@ -4931,16 +4950,16 @@
     </row>
     <row r="141" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B141" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C141" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D141" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C141" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D141" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="E141" s="6" t="s">
         <v>23</v>
@@ -4960,16 +4979,16 @@
     </row>
     <row r="142" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B142" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C142" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D142" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="C142" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D142" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="E142" s="6" t="s">
         <v>23</v>
@@ -4989,16 +5008,16 @@
     </row>
     <row r="143" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B143" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C143" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D143" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C143" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D143" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="E143" s="6" t="s">
         <v>23</v>
@@ -5018,12 +5037,12 @@
     </row>
     <row r="144" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B144" s="30"/>
       <c r="C144" s="4"/>
       <c r="D144" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E144" s="4"/>
       <c r="F144" s="4"/>
@@ -5035,19 +5054,19 @@
     </row>
     <row r="145" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B145" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D145" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C145" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D145" s="7" t="s">
+      <c r="E145" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="E145" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="F145" s="6">
         <v>12</v>
@@ -5064,16 +5083,16 @@
     </row>
     <row r="146" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B146" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D146" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C146" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D146" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="E146" s="6" t="s">
         <v>23</v>
@@ -5093,16 +5112,16 @@
     </row>
     <row r="147" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B147" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C147" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D147" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C147" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D147" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="E147" s="6" t="s">
         <v>23</v>
@@ -5122,19 +5141,19 @@
     </row>
     <row r="148" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B148" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D148" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C148" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D148" s="7" t="s">
+      <c r="E148" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="E148" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="F148" s="6">
         <v>3.6</v>
@@ -5151,12 +5170,12 @@
     </row>
     <row r="149" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B149" s="30"/>
       <c r="C149" s="4"/>
       <c r="D149" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E149" s="4"/>
       <c r="F149" s="4"/>
@@ -5168,12 +5187,12 @@
     </row>
     <row r="150" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B150" s="29"/>
       <c r="C150" s="2"/>
       <c r="D150" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E150" s="2"/>
       <c r="F150" s="2"/>
@@ -5185,16 +5204,16 @@
     </row>
     <row r="151" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B151" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C151" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D151" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="C151" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D151" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="E151" s="6" t="s">
         <v>23</v>
@@ -5214,16 +5233,16 @@
     </row>
     <row r="152" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B152" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C152" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D152" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="C152" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D152" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="E152" s="6" t="s">
         <v>23</v>
@@ -5243,16 +5262,16 @@
     </row>
     <row r="153" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B153" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D153" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="C153" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D153" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="E153" s="6" t="s">
         <v>23</v>
@@ -5272,12 +5291,12 @@
     </row>
     <row r="154" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B154" s="30"/>
       <c r="C154" s="4"/>
       <c r="D154" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E154" s="4"/>
       <c r="F154" s="4"/>
@@ -5289,7 +5308,7 @@
     </row>
     <row r="155" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B155" s="25" t="s">
         <v>31</v>
@@ -5318,16 +5337,16 @@
     </row>
     <row r="156" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B156" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C156" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D156" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C156" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D156" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="E156" s="6" t="s">
         <v>23</v>
@@ -5347,16 +5366,16 @@
     </row>
     <row r="157" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B157" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C157" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D157" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="C157" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D157" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="E157" s="6" t="s">
         <v>23</v>
@@ -5376,16 +5395,16 @@
     </row>
     <row r="158" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B158" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C158" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D158" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C158" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D158" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="E158" s="6" t="s">
         <v>23</v>
@@ -5405,12 +5424,12 @@
     </row>
     <row r="159" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B159" s="30"/>
       <c r="C159" s="4"/>
       <c r="D159" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E159" s="4"/>
       <c r="F159" s="4"/>
@@ -5422,19 +5441,19 @@
     </row>
     <row r="160" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B160" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C160" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D160" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C160" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D160" s="7" t="s">
+      <c r="E160" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="E160" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="F160" s="6">
         <v>12</v>
@@ -5451,16 +5470,16 @@
     </row>
     <row r="161" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B161" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C161" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D161" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C161" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D161" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="E161" s="6" t="s">
         <v>23</v>
@@ -5480,16 +5499,16 @@
     </row>
     <row r="162" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B162" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C162" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D162" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C162" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D162" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="E162" s="6" t="s">
         <v>23</v>
@@ -5509,19 +5528,19 @@
     </row>
     <row r="163" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B163" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D163" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C163" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D163" s="7" t="s">
+      <c r="E163" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="E163" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="F163" s="6">
         <v>3.6</v>
@@ -5548,49 +5567,49 @@
       <c r="I164" s="21"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A165" s="35"/>
-      <c r="B165" s="35"/>
-      <c r="C165" s="35"/>
+      <c r="A165" s="36"/>
+      <c r="B165" s="36"/>
+      <c r="C165" s="36"/>
       <c r="D165" s="22"/>
       <c r="E165" s="10"/>
-      <c r="F165" s="34" t="s">
-        <v>221</v>
-      </c>
-      <c r="G165" s="35"/>
-      <c r="H165" s="36">
+      <c r="F165" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="G165" s="36"/>
+      <c r="H165" s="38">
         <v>1945452.28</v>
       </c>
-      <c r="I165" s="35"/>
+      <c r="I165" s="36"/>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A166" s="35"/>
-      <c r="B166" s="35"/>
-      <c r="C166" s="35"/>
+      <c r="A166" s="36"/>
+      <c r="B166" s="36"/>
+      <c r="C166" s="36"/>
       <c r="D166" s="22"/>
       <c r="E166" s="10"/>
-      <c r="F166" s="34" t="s">
-        <v>222</v>
-      </c>
-      <c r="G166" s="35"/>
-      <c r="H166" s="36">
+      <c r="F166" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="G166" s="36"/>
+      <c r="H166" s="38">
         <v>0</v>
       </c>
-      <c r="I166" s="35"/>
+      <c r="I166" s="36"/>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A167" s="35"/>
-      <c r="B167" s="35"/>
-      <c r="C167" s="35"/>
+      <c r="A167" s="36"/>
+      <c r="B167" s="36"/>
+      <c r="C167" s="36"/>
       <c r="D167" s="22"/>
       <c r="E167" s="10"/>
-      <c r="F167" s="34" t="s">
-        <v>223</v>
-      </c>
-      <c r="G167" s="35"/>
-      <c r="H167" s="36">
+      <c r="F167" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="G167" s="36"/>
+      <c r="H167" s="38">
         <v>1945452.28</v>
       </c>
-      <c r="I167" s="35"/>
+      <c r="I167" s="36"/>
     </row>
     <row r="168" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="10"/>
@@ -5604,20 +5623,27 @@
       <c r="I168" s="23"/>
     </row>
     <row r="169" spans="1:9" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="B169" s="38"/>
-      <c r="C169" s="38"/>
-      <c r="D169" s="38"/>
-      <c r="E169" s="38"/>
-      <c r="F169" s="38"/>
-      <c r="G169" s="38"/>
-      <c r="H169" s="38"/>
-      <c r="I169" s="38"/>
+      <c r="A169" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="B169" s="34"/>
+      <c r="C169" s="34"/>
+      <c r="D169" s="34"/>
+      <c r="E169" s="34"/>
+      <c r="F169" s="34"/>
+      <c r="G169" s="34"/>
+      <c r="H169" s="34"/>
+      <c r="I169" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A167:C167"/>
+    <mergeCell ref="F167:G167"/>
+    <mergeCell ref="H167:I167"/>
     <mergeCell ref="A169:I169"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A165:C165"/>
@@ -5626,13 +5652,6 @@
     <mergeCell ref="A166:C166"/>
     <mergeCell ref="F166:G166"/>
     <mergeCell ref="H166:I166"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A167:C167"/>
-    <mergeCell ref="F167:G167"/>
-    <mergeCell ref="H167:I167"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>